<commit_message>
Fix defined names conversion
</commit_message>
<xml_diff>
--- a/OOXML/test/ExampleFiles/xlsx2xlsb/simple2.xlsx
+++ b/OOXML/test/ExampleFiles/xlsx2xlsb/simple2.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr allowRefreshQuery="0" autoCompressPictures="1" backupFile="0" checkCompatibility="0" codeName="0" date1904="0" dateCompatibility="1" defaultThemeVersion="0" filterPrivacy="0" hidePivotFieldList="0" promptedSolutions="0" publishItems="0" refreshAllConnections="0" showBorderUnselectedTables="0" showInkAnnotation="1" showObjects="all" showPivotChartFilter="0" updateLinks="always"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId4"/>
+    <sheet name="Лист2" sheetId="2" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="Slicer_it">#N/A</definedName>
+    <definedName name="Slicer_it" hidden="0">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="0" calcMode="autoNoTable" fullCalcOnLoad="0" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001" fullPrecision="1" calcCompleted="0" calcOnSave="1" concurrentCalc="1" concurrentManualCount="1" forceFullCalc="0"/>
+  <calcPr/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId1"/>
   </pivotCaches>
   <extLst>
-    <ext uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
-      <x15:slicerCaches>
-        <x14:slicerCache r:id="rId4"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
+      <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:slicerCache r:id="rId2"/>
       </x15:slicerCaches>
     </ext>
   </extLst>
@@ -32,11 +32,25 @@
     <author>tc={5A175D1A-2D6E-3CC8-2227-22732FCB5686}</author>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0" xr:uid="{00000000-0000-0000-0000-000000000000}">
+    <comment ref="D4" authorId="0" xr:uid="{5A175D1A-2D6E-3CC8-2227-22732FCB5686}">
       <text>
-        <t xml:space="preserve">Vik:
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Vik:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
 test comment
 </t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -68,107 +82,44 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="1">
     <font>
-      <i val="0"/>
-      <strike val="0"/>
-      <condense val="0"/>
-      <extend val="0"/>
-      <outline val="0"/>
-      <shadow val="0"/>
-      <u val="none"/>
-      <vertAlign val="baseline"/>
       <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <condense val="0"/>
-      <extend val="0"/>
-      <outline val="0"/>
-      <shadow val="0"/>
-      <u val="none"/>
-      <vertAlign val="baseline"/>
-      <sz val="9.000000"/>
-      <color auto="1"/>
-      <name val="Tahoma"/>
-      <family val="0"/>
-      <charset val="0"/>
-      <scheme val="none"/>
-    </font>
-    <font>
-      <i val="0"/>
-      <strike val="0"/>
-      <condense val="0"/>
-      <extend val="0"/>
-      <outline val="0"/>
-      <shadow val="0"/>
-      <u val="none"/>
-      <vertAlign val="baseline"/>
-      <sz val="9.000000"/>
-      <color auto="1"/>
-      <name val="Tahoma"/>
-      <family val="0"/>
-      <charset val="0"/>
-      <scheme val="none"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="64"/>
-        <bgColor indexed="65"/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor indexed="64"/>
-        <bgColor indexed="65"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
     <border>
-      <left style="none">
-        <color auto="1"/>
-      </left>
-      <right style="none">
-        <color auto="1"/>
-      </right>
-      <top style="none">
-        <color auto="1"/>
-      </top>
-      <bottom style="none">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="none">
-        <color auto="1"/>
-      </diagonal>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" quotePrefix="0" pivotButton="0">
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" relativeIndent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" quotePrefix="0" pivotButton="0">
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" relativeIndent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43E5-95BD-54CBDDF9020C}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
@@ -182,16 +133,16 @@
     <xdr:ext cx="1828800" cy="2523742"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
-        <xdr:graphicFrame macro="">
+        <xdr:graphicFrame>
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="294272694" name="it"/>
+            <xdr:cNvPr id="294272694" name=""/>
             <xdr:cNvGraphicFramePr>
               <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
             </xdr:cNvGraphicFramePr>
           </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
+          <xdr:xfrm rot="0" flipH="0" flipV="0">
+            <a:off x="6420823" y="777451"/>
+            <a:ext cx="1828800" cy="2523743"/>
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
@@ -251,28 +202,23 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" r:id="rId1" refreshedDateIso="0.000000" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="2">
-  <cacheSource connectionId="0" type="worksheet">
-    <worksheetSource sheet="Лист1" ref="C6:D8"/>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="2">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="C6:D8" sheet="Лист1"/>
   </cacheSource>
   <cacheFields count="2">
-    <cacheField name="1" mappingCount="0" numFmtId="-1">
-      <sharedItems count="0" containsBlank="0" containsDate="0" containsInteger="1" containsMixedTypes="0" containsNonDate="1" containsNumber="1" containsSemiMixedTypes="0" containsString="0" longText="0" minValue="8" maxValue="178"/>
+    <cacheField name="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="8" maxValue="178"/>
     </cacheField>
-    <cacheField name="4" mappingCount="0" numFmtId="-1">
-      <sharedItems count="0" containsBlank="0" containsDate="0" containsInteger="1" containsMixedTypes="0" containsNonDate="1" containsNumber="1" containsSemiMixedTypes="0" containsString="0" longText="0" minValue="9" maxValue="87"/>
+    <cacheField name="4">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="9" maxValue="87"/>
     </cacheField>
   </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition pivotCacheId="0"/>
-    </ext>
-  </extLst>
 </pivotCacheDefinition>
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" count="2">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="2">
   <r>
     <n v="8"/>
     <n v="9"/>
@@ -285,52 +231,342 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="PivotTable1" cacheId="0" dataCaption="Значения" applyAlignmentFormats="0" applyBorderFormats="0" applyFontFormats="0" applyNumberFormats="0" applyPatternFormats="0" applyWidthHeightFormats="1" autoFormatId="1" createdVersion="4" immersive="0" indent="0" itemPrintTitles="1" minRefreshableVersion="3" multipleFieldFilters="0" outline="1" outlineData="1" updatedVersion="4" useAutoFormatting="1" visualTotals="0">
-  <location colPageCount="0" firstDataCol="0" firstDataRow="2" firstHeaderRow="1" ref="A3:B5" rowPageCount="0"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B5" firstHeaderRow="1" firstDataRow="2" firstDataCol="0"/>
   <pivotFields count="2">
-    <pivotField dataField="1" dataSourceSort="0" includeNewItemsInFilter="1" showAll="0" axis="axisValues" sortType="manual" numFmtId="0"/>
-    <pivotField dataField="1" dataSourceSort="0" includeNewItemsInFilter="1" showAll="0" axis="axisValues" sortType="manual" numFmtId="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowItems count="1">
-    <i i="0" r="0" t="data"/>
+    <i/>
   </rowItems>
   <colFields count="1">
     <field x="-2"/>
   </colFields>
   <colItems count="2">
-    <i i="0" r="0" t="data">
-      <x v="0"/>
+    <i>
+      <x/>
     </i>
-    <i i="1" r="0" t="data">
+    <i i="1">
       <x v="1"/>
     </i>
   </colItems>
   <dataFields count="2">
-    <dataField name="Sum of 1" baseField="0" baseItem="0" fld="0" numFmtId="0"/>
-    <dataField name="Sum of 4" baseField="0" baseItem="0" fld="1" numFmtId="0"/>
+    <dataField name="Sum of 1" fld="0" baseField="0" baseItem="0"/>
+    <dataField name="Sum of 4" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showColHeaders="1" showColStripes="0" showLastColumn="1" showRowHeaders="1" showRowStripes="0"/>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
 </pivotTableDefinition>
 </file>
 
-<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?><slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x xr10" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" name="Slicer_it" sourceName="it"><extLst><ext uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}"><x15:tableSlicerCache tableId="1" column="1" sortOrder="ascending" customListSort="1" crossFilter="showItemsWithDataAtTop"></x15:tableSlicerCache></ext></extLst></slicerCacheDefinition>
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_it" xr10:uid="{E69683C1-E062-A9E6-F35A-4CFB7BCB314B}" sourceName="it">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="1" column="1" sortOrder="ascending" customListSort="1" crossFilter="showItemsWithDataAtTop"/>
+    </ext>
+  </extLst>
+</slicerCacheDefinition>
 </file>
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
-  <slicer name="it" xr10:uid="it" cache="Slicer_it" caption="it" startItem="0" columnCount="1" showCaption="1" level="0" lockedPosition="0" rowHeight="241300"/>
+  <slicer name="it" xr10:uid="{982EC51D-07DE-91A4-1DAB-70F24D5E7F96}" cache="Slicer_it" caption="it" startItem="0" columnCount="1" showCaption="1" level="0" lockedPosition="0" rowHeight="241300"/>
 </slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="Таблица1" displayName="Таблица1" ref="B1:C4" connectionId="0" tableType="worksheet" totalsRowShown="1" insertRow="0" insertRowShift="0" published="0">
-  <autoFilter ref="B1:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Таблица1" ref="$B$1:$C$4">
+  <autoFilter ref="$B$1:$C$4"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="it" totalsRowFunction="none" queryTableFieldId="0"/>
-    <tableColumn id="2" name="ut" totalsRowFunction="none" queryTableFieldId="0"/>
+    <tableColumn id="1" name="it"/>
+    <tableColumn id="2" name="ut"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
+</file>
+
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -341,7 +577,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -551,140 +787,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr syncHorizontal="0" syncVertical="0" transitionEvaluation="0" transitionEntry="0" published="1" filterMode="0" enableFormatConditionsCalculation="0">
-    <tabColor auto="1"/>
-    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
-  </sheetPr>
   <sheetViews>
-    <sheetView windowProtection="0" showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" showWhiteSpace="0" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col bestFit="1" collapsed="0" customWidth="0" hidden="0" min="1" max="1" outlineLevel="0" phonetic="0" style="0" width="9.36328125"/>
-    <col bestFit="1" collapsed="0" customWidth="0" hidden="0" min="2" max="2" outlineLevel="0" phonetic="0" style="0" width="8.54296875"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="3" ht="14.5">
+    <row r="1" ht="14.25">
+      <c r="A1">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" ht="14.5">
-      <c r="A4" t="s">
+    <row r="4" ht="14.25">
+      <c r="B4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="5" ht="14.5">
-      <c r="A5">
-        <v>186</v>
-      </c>
-      <c r="B5">
-        <v>96</v>
+    <row r="7" ht="14.25">
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="C8">
+        <v>178</v>
+      </c>
+      <c r="D8">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="0" autoFilter="0" content="1" deleteColumns="0" deleteRows="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertHyperlinks="0" insertRows="0" objects="1" pivotTables="0" scenarios="1" selectLockedCells="1" selectUnlockedCells="1" sheet="0" sort="0"/>
-  <printOptions headings="0" gridLines="0" gridLinesSet="0" horizontalCentered="0" verticalCentered="0"/>
+  <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1" r:id=""/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr syncHorizontal="0" syncVertical="0" transitionEvaluation="0" transitionEntry="0" published="1" filterMode="0" enableFormatConditionsCalculation="0">
-    <tabColor auto="1"/>
-    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView windowProtection="0" showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" showWhiteSpace="0" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" ht="14.5">
-      <c r="A1">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" ht="14.5">
-      <c r="A2">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" ht="14.5">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" ht="14.5">
-      <c r="B4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" ht="14.5">
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" ht="14.5">
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" ht="14.5">
-      <c r="C8">
-        <v>178</v>
-      </c>
-      <c r="D8">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection password="0" autoFilter="0" content="1" deleteColumns="0" deleteRows="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertHyperlinks="0" insertRows="0" objects="1" pivotTables="0" scenarios="1" selectLockedCells="1" selectUnlockedCells="1" sheet="0" sort="0"/>
-  <printOptions headings="0" gridLines="0" gridLinesSet="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1" r:id=""/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
   <extLst>
-    <ext uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
       <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicer r:id="rId5"/>
+        <x14:slicer r:id="rId6"/>
       </x14:slicerList>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="9.3828125"/>
+    <col bestFit="1" min="2" max="2" width="8.5234375"/>
+  </cols>
+  <sheetData>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>186</v>
+      </c>
+      <c r="B5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>